<commit_message>
need to finish currency filter
</commit_message>
<xml_diff>
--- a/reports/Test_Report.xlsx
+++ b/reports/Test_Report.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Results" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,22 +24,13 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DDDDDD"/>
-        <bgColor rgb="00DDDDDD"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,14 +45,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -141,10 +134,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -182,69 +175,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -268,54 +263,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -325,7 +319,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -334,7 +328,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -343,7 +337,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -351,10 +345,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -383,7 +377,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -396,13 +390,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -422,40 +415,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="27.43357142857143" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="23.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="7.719285714285714" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="97.57642857142856" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Page URL</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Test Case</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Comments</t>
         </is>
@@ -535,17 +528,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>H1 Tag Existence</t>
+          <t>Currency Filtering</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>H1 tag found</t>
+          <t>Error during currency filtering: 'mismatched'</t>
         </is>
       </c>
     </row>
@@ -557,17 +550,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HTML Tag Sequence</t>
+          <t>Script Data Scraping</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Invalid sequence: ['h5', 'h1', 'h6', 'h6', 'h6', 'h6', 'h6', 'h6', 'h6', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h2', 'h4', 'h4', 'h4', 'h4', 'h4']</t>
+          <t>Scraped data: {'SiteURL': '', 'CampaignID': '', 'SiteName': '', 'Browser': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/131.0.0.0 Safari/537.36', 'CountryCode': '', 'IP': ''}</t>
         </is>
       </c>
     </row>
@@ -579,7 +572,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Image Alt Attributes</t>
+          <t>Script Data Scraping</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -589,11 +582,55 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>All images have alt attributes</t>
+          <t>Scraped data: {'SiteURL': '', 'CampaignID': '', 'SiteName': '', 'Browser': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/131.0.0.0 Safari/537.36', 'CountryCode': '', 'IP': ''}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Script Data Scraping</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Scraped data: {'SiteURL': '', 'CampaignID': '', 'SiteName': '', 'Browser': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/131.0.0.0 Safari/537.36', 'CountryCode': '', 'IP': ''}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Script Data Scraping</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Scraped data: {'SiteURL': '', 'CampaignID': '', 'SiteName': '', 'Browser': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/131.0.0.0 Safari/537.36', 'CountryCode': '', 'IP': ''}</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>